<commit_message>
Reorganize the match from industries to patents
</commit_message>
<xml_diff>
--- a/conversion_patent2industry/industry_names.xlsx
+++ b/conversion_patent2industry/industry_names.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>311</t>
   </si>
@@ -196,9 +196,6 @@
     <t xml:space="preserve">Other Miscellaneous                                                             </t>
   </si>
   <si>
-    <t xml:space="preserve">All Industries               </t>
-  </si>
-  <si>
     <t>313+</t>
   </si>
   <si>
@@ -230,9 +227,6 @@
   </si>
   <si>
     <t>339-</t>
-  </si>
-  <si>
-    <t>R5</t>
   </si>
 </sst>
 </file>
@@ -268,9 +262,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,9 +567,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="A31:XFD31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -583,7 +580,7 @@
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -593,8 +590,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -604,10 +604,13 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>32</v>
@@ -615,8 +618,11 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -626,10 +632,13 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>34</v>
@@ -637,10 +646,13 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>
@@ -648,8 +660,11 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -659,8 +674,11 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -670,8 +688,11 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -681,10 +702,13 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>39</v>
@@ -692,8 +716,11 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -703,8 +730,11 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -714,8 +744,11 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -725,8 +758,11 @@
       <c r="C13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -736,8 +772,11 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -747,10 +786,13 @@
       <c r="C15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>45</v>
@@ -758,8 +800,11 @@
       <c r="C16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -769,8 +814,11 @@
       <c r="C17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -780,8 +828,11 @@
       <c r="C18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -791,8 +842,11 @@
       <c r="C19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -802,10 +856,13 @@
       <c r="C20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>50</v>
@@ -813,8 +870,11 @@
       <c r="C21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -824,10 +884,13 @@
       <c r="C22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>52</v>
@@ -835,10 +898,13 @@
       <c r="C23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>53</v>
@@ -846,8 +912,11 @@
       <c r="C24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -857,10 +926,13 @@
       <c r="C25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>55</v>
@@ -868,8 +940,11 @@
       <c r="C26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -879,10 +954,13 @@
       <c r="C27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>57</v>
@@ -890,8 +968,11 @@
       <c r="C28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -901,10 +982,13 @@
       <c r="C29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>59</v>
@@ -912,15 +996,9 @@
       <c r="C30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="1"/>
+      <c r="D30" s="2">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
In bilateral plot, color industries according to industry groups
</commit_message>
<xml_diff>
--- a/conversion_patent2industry/industry_names.xlsx
+++ b/conversion_patent2industry/industry_names.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
   <si>
     <t>311</t>
   </si>
@@ -31,9 +31,6 @@
     <t>322,323</t>
   </si>
   <si>
-    <t>325</t>
-  </si>
-  <si>
     <t>3251</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>333</t>
   </si>
   <si>
-    <t>334</t>
-  </si>
-  <si>
     <t>3341</t>
   </si>
   <si>
@@ -82,9 +76,6 @@
     <t>335</t>
   </si>
   <si>
-    <t>336</t>
-  </si>
-  <si>
     <t>3361-3363</t>
   </si>
   <si>
@@ -97,9 +88,6 @@
     <t>337</t>
   </si>
   <si>
-    <t>339</t>
-  </si>
-  <si>
     <t>3391</t>
   </si>
   <si>
@@ -121,9 +109,6 @@
     <t xml:space="preserve">Paper, Printing and support activities                                          </t>
   </si>
   <si>
-    <t xml:space="preserve">Chemicals                                                                       </t>
-  </si>
-  <si>
     <t xml:space="preserve">Basic Chemicals                                                                 </t>
   </si>
   <si>
@@ -151,9 +136,6 @@
     <t xml:space="preserve">Machinery                                                                       </t>
   </si>
   <si>
-    <t xml:space="preserve">Computer and Electronic Products                                                </t>
-  </si>
-  <si>
     <t xml:space="preserve">Computer and Peripheral Equipment                                               </t>
   </si>
   <si>
@@ -172,9 +154,6 @@
     <t xml:space="preserve">Electrical Equipment, Appliances, and Components                                </t>
   </si>
   <si>
-    <t xml:space="preserve">Transportation Equipment                                                        </t>
-  </si>
-  <si>
     <t xml:space="preserve">Motor Vehicles, Trailers and Parts                                              </t>
   </si>
   <si>
@@ -187,9 +166,6 @@
     <t xml:space="preserve">Furniture and Related Products                                                  </t>
   </si>
   <si>
-    <t xml:space="preserve">Miscellaneous Manufacturing                                                     </t>
-  </si>
-  <si>
     <t xml:space="preserve">Medical Equipment and Supplies                                                  </t>
   </si>
   <si>
@@ -202,28 +178,16 @@
     <t>322+</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
     <t>325-</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
     <t>334-</t>
   </si>
   <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>3361+</t>
   </si>
   <si>
     <t>336-</t>
-  </si>
-  <si>
-    <t>R4</t>
   </si>
   <si>
     <t>339-</t>
@@ -567,11 +531,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="A31:XFD31"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -585,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -599,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -610,10 +572,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -627,7 +589,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -638,10 +600,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -652,10 +614,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -669,7 +631,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -683,35 +645,35 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -725,13 +687,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -739,7 +701,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -753,7 +715,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -767,7 +729,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -781,21 +743,21 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -809,7 +771,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -823,7 +785,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -834,10 +796,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -851,7 +813,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
@@ -862,16 +824,16 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,21 +841,21 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
         <v>22</v>
@@ -904,16 +866,16 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="2">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,82 +883,26 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
       </c>
       <c r="D26" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="2">
         <v>10</v>
       </c>
     </row>

</xml_diff>